<commit_message>
[Doc]_Update tiến độ các task
</commit_message>
<xml_diff>
--- a/WIP/Users/HuyenPT/Tiến độ các task  của dự án.xlsx
+++ b/WIP/Users/HuyenPT/Tiến độ các task  của dự án.xlsx
@@ -12,10 +12,10 @@
     <sheet name="TESTING" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CODING!$K$4:$K$84</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CODING!$H$10:$H$82</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">DESIGN!$I$4:$I$17</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TESTING!$H$4:$H$17</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">CODING!$A$4:$O$74</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">CODING!$A$10:$M$80</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">DESIGN!$A$7:$L$8</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">TESTING!$A$4:$K$8</definedName>
   </definedNames>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="267">
   <si>
     <t>Use Case No.</t>
   </si>
@@ -764,22 +764,12 @@
     <t>25/10/2019</t>
   </si>
   <si>
-    <t>ghép giao diện</t>
-  </si>
-  <si>
     <t>cấm 1 nhóm</t>
   </si>
   <si>
     <t>gỡ bỏ lệnh cấm nhóm</t>
   </si>
   <si>
-    <t>hết 8/11</t>
-  </si>
-  <si>
-    <t>9/11 bắt đầu
-hiển thị trang cá nhân</t>
-  </si>
-  <si>
     <t>Screen Design</t>
   </si>
   <si>
@@ -802,13 +792,46 @@
   </si>
   <si>
     <t>Unban a group</t>
+  </si>
+  <si>
+    <t>Ghép giao diện</t>
+  </si>
+  <si>
+    <t>chưa có button đăng xuất</t>
+  </si>
+  <si>
+    <t>chờ done rating</t>
+  </si>
+  <si>
+    <t>vào trang của book mới rate được</t>
+  </si>
+  <si>
+    <t>Chờ done phần search</t>
+  </si>
+  <si>
+    <t>bỏ</t>
+  </si>
+  <si>
+    <t>màu đỏ</t>
+  </si>
+  <si>
+    <t>màu vàng</t>
+  </si>
+  <si>
+    <t>độ ưu tiên cao</t>
+  </si>
+  <si>
+    <t>màu xanh</t>
+  </si>
+  <si>
+    <t>các phần có làm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -859,8 +882,15 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -939,6 +969,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1047,7 +1095,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1156,6 +1204,14 @@
     <xf numFmtId="14" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1168,15 +1224,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1189,6 +1236,30 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="11" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1201,6 +1272,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1210,15 +1296,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1228,27 +1305,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1264,23 +1320,89 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1585,7 +1707,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:O76"/>
+  <dimension ref="A1:M82"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
@@ -1600,914 +1722,833 @@
     <col min="7" max="7" width="50.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="15.5703125" style="19" customWidth="1"/>
     <col min="11" max="11" width="12.42578125" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" style="94" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:14" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="D4" s="2" t="s">
+    <row r="1" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="L1" s="94"/>
+    </row>
+    <row r="3" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="116" t="s">
+        <v>262</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="I3" s="50">
+        <f>COUNTIF(K13:K83,"Done")</f>
+        <v>23</v>
+      </c>
+      <c r="J3" s="19"/>
+      <c r="L3" s="94"/>
+    </row>
+    <row r="4" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="117" t="s">
+        <v>263</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="I4" s="49">
+        <f>COUNTIF(K13:K82,"In Progress")</f>
+        <v>18</v>
+      </c>
+      <c r="J4" s="19"/>
+      <c r="L4" s="94"/>
+    </row>
+    <row r="5" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="118" t="s">
+        <v>265</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="I5" s="12">
+        <f>COUNTIF(K13:K82, "Not Start")</f>
+        <v>11</v>
+      </c>
+      <c r="J5" s="19"/>
+      <c r="L5" s="94"/>
+    </row>
+    <row r="6" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H6" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="I6" s="12">
+        <f>SUM(I3:I5)</f>
+        <v>52</v>
+      </c>
+      <c r="J6" s="19"/>
+      <c r="L6" s="94"/>
+    </row>
+    <row r="7" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="L7" s="94"/>
+    </row>
+    <row r="10" spans="2:12" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="D10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J10" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K10" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="M4" s="48" t="s">
-        <v>215</v>
-      </c>
-      <c r="N4" s="48"/>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D5" s="62" t="s">
+      <c r="L10" s="95" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D11" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="12"/>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D6" s="75" t="s">
+      <c r="E11" s="71"/>
+      <c r="F11" s="71"/>
+      <c r="G11" s="71"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="96"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D12" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="75"/>
-      <c r="F6" s="75"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="12"/>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="E12" s="73"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="73"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="96"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>209</v>
       </c>
-      <c r="D7" s="72" t="s">
+      <c r="D13" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="72" t="s">
+      <c r="E13" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F13" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G13" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="27"/>
-      <c r="M7" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="N7" s="90">
-        <f>COUNTIF(K5:K76,"Done")</f>
+      <c r="H13" s="92"/>
+      <c r="I13" s="92"/>
+      <c r="J13" s="92"/>
+      <c r="K13" s="93"/>
+      <c r="L13" s="97"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>210</v>
+      </c>
+      <c r="D14" s="66"/>
+      <c r="E14" s="66"/>
+      <c r="F14" s="88" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="88" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="92"/>
+      <c r="I14" s="92"/>
+      <c r="J14" s="92"/>
+      <c r="K14" s="93"/>
+      <c r="L14" s="97"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>205</v>
+      </c>
+      <c r="D15" s="67"/>
+      <c r="E15" s="66"/>
+      <c r="F15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="I15" s="24" t="s">
+        <v>238</v>
+      </c>
+      <c r="J15" s="24" t="s">
+        <v>242</v>
+      </c>
+      <c r="K15" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="L15" s="98" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="D16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="67"/>
+      <c r="F16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>210</v>
-      </c>
-      <c r="D8" s="74"/>
-      <c r="E8" s="74"/>
-      <c r="F8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="27"/>
-      <c r="M8" s="15" t="s">
+      <c r="H16" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="I16" s="24" t="s">
+        <v>239</v>
+      </c>
+      <c r="J16" s="24" t="s">
+        <v>243</v>
+      </c>
+      <c r="K16" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="L16" s="99" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="I17" s="24" t="s">
+        <v>240</v>
+      </c>
+      <c r="J17" s="24" t="s">
+        <v>244</v>
+      </c>
+      <c r="K17" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="L17" s="98" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="67"/>
+      <c r="F18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="I18" s="24" t="s">
+        <v>241</v>
+      </c>
+      <c r="J18" s="24" t="s">
+        <v>245</v>
+      </c>
+      <c r="K18" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="L18" s="98" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="18" t="s">
         <v>207</v>
       </c>
-      <c r="N8" s="89">
-        <f>COUNTIF(K8:K94,"In Progress")</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="D19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19" s="24" t="s">
         <v>205</v>
       </c>
-      <c r="D9" s="73"/>
-      <c r="E9" s="74"/>
-      <c r="F9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="24" t="s">
-        <v>205</v>
-      </c>
-      <c r="I9" s="24" t="s">
-        <v>238</v>
-      </c>
-      <c r="J9" s="24" t="s">
-        <v>242</v>
-      </c>
-      <c r="K9" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="L9" s="87"/>
-      <c r="M9" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="N9" s="12">
-        <f>COUNTIF(K6:K78, "Not Start")</f>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="73"/>
-      <c r="F10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" s="24" t="s">
-        <v>205</v>
-      </c>
-      <c r="I10" s="24" t="s">
-        <v>239</v>
-      </c>
-      <c r="J10" s="24" t="s">
-        <v>243</v>
-      </c>
-      <c r="K10" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="M10" s="12" t="s">
-        <v>216</v>
-      </c>
-      <c r="N10" s="12">
-        <f>SUM(N7:N9)</f>
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="72" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="24" t="s">
-        <v>205</v>
-      </c>
-      <c r="I11" s="24" t="s">
-        <v>240</v>
-      </c>
-      <c r="J11" s="24" t="s">
-        <v>244</v>
-      </c>
-      <c r="K11" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="M11" s="21"/>
-      <c r="N11" s="21"/>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="73"/>
-      <c r="F12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" s="24" t="s">
-        <v>205</v>
-      </c>
-      <c r="I12" s="24" t="s">
-        <v>241</v>
-      </c>
-      <c r="J12" s="24" t="s">
-        <v>245</v>
-      </c>
-      <c r="K12" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="M12" s="21" t="s">
-        <v>210</v>
-      </c>
-      <c r="N12" s="21">
-        <f>COUNTIF(H5:H88,"DangVH")</f>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="18" t="s">
-        <v>207</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13" s="24" t="s">
-        <v>205</v>
-      </c>
-      <c r="I13" s="85">
+      <c r="I19" s="48">
         <v>42593</v>
       </c>
-      <c r="J13" s="24"/>
-      <c r="K13" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="M13" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="N13" s="21">
-        <f>COUNTIF(H6:H89,"HuyenPT")</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="17" t="s">
-        <v>206</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H14" s="24" t="s">
-        <v>205</v>
-      </c>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="M14" s="21" t="s">
-        <v>205</v>
-      </c>
-      <c r="N14" s="21">
-        <f>COUNTIF(H7:H90,"VanTTC")</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D15" s="76" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" s="77"/>
-      <c r="F15" s="77"/>
-      <c r="G15" s="78"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="12"/>
-    </row>
-    <row r="16" spans="2:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="D16" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="72" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H16" s="25" t="s">
-        <v>209</v>
-      </c>
-      <c r="I16" s="47">
-        <v>42562</v>
-      </c>
-      <c r="J16" s="25"/>
-      <c r="K16" s="15" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="17" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D17" s="72" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="74"/>
-      <c r="F17" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H17" s="55" t="s">
-        <v>209</v>
-      </c>
-      <c r="I17" s="47">
-        <v>42562</v>
-      </c>
-      <c r="J17" s="28"/>
-      <c r="K17" s="57" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="18" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D18" s="73"/>
-      <c r="E18" s="74"/>
-      <c r="F18" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H18" s="56"/>
-      <c r="I18" s="47">
-        <v>42562</v>
-      </c>
-      <c r="J18" s="29"/>
-      <c r="K18" s="58"/>
-    </row>
-    <row r="19" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D19" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E19" s="74"/>
-      <c r="F19" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H19" s="25" t="s">
-        <v>209</v>
-      </c>
-      <c r="I19" s="47">
-        <v>42562</v>
-      </c>
-      <c r="J19" s="25"/>
+      <c r="J19" s="24"/>
       <c r="K19" s="15" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="20" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D20" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" s="74"/>
+      <c r="L19" s="100"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B20" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="4"/>
       <c r="F20" s="3" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="13" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="21" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D21" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E21" s="73"/>
-      <c r="F21" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>47</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="L20" s="98" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D21" s="74" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="75"/>
+      <c r="F21" s="75"/>
+      <c r="G21" s="76"/>
       <c r="H21" s="22"/>
       <c r="I21" s="22"/>
       <c r="J21" s="22"/>
-      <c r="K21" s="13" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="22" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="K21" s="12"/>
+      <c r="L21" s="96"/>
+    </row>
+    <row r="22" spans="2:13" ht="45" x14ac:dyDescent="0.25">
       <c r="D22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="90" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" s="91" t="s">
+        <v>33</v>
+      </c>
+      <c r="H22" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="I22" s="47">
+        <v>42562</v>
+      </c>
+      <c r="J22" s="25"/>
+      <c r="K22" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="L22" s="98" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D23" s="65" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="66"/>
+      <c r="F23" s="90" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" s="90" t="s">
+        <v>36</v>
+      </c>
+      <c r="H23" s="56" t="s">
+        <v>209</v>
+      </c>
+      <c r="I23" s="60"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="58" t="s">
+        <v>207</v>
+      </c>
+      <c r="L23" s="101"/>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D24" s="67"/>
+      <c r="E24" s="66"/>
+      <c r="F24" s="90" t="s">
+        <v>37</v>
+      </c>
+      <c r="G24" s="90" t="s">
+        <v>38</v>
+      </c>
+      <c r="H24" s="57"/>
+      <c r="I24" s="61"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="59"/>
+      <c r="L24" s="102"/>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D25" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" s="66"/>
+      <c r="F25" s="90" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="90" t="s">
+        <v>41</v>
+      </c>
+      <c r="H25" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="I25" s="47"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="L25" s="100"/>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D26" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26" s="66"/>
+      <c r="F26" s="90" t="s">
+        <v>43</v>
+      </c>
+      <c r="G26" s="90" t="s">
+        <v>44</v>
+      </c>
+      <c r="H26" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="I26" s="47"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="L26" s="100"/>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D27" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" s="67"/>
+      <c r="F27" s="90" t="s">
+        <v>46</v>
+      </c>
+      <c r="G27" s="90" t="s">
+        <v>47</v>
+      </c>
+      <c r="H27" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="I27" s="47"/>
+      <c r="J27" s="25"/>
+      <c r="K27" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="L27" s="100"/>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D28" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E22" s="72" t="s">
+      <c r="E28" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F28" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G28" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="13" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="23" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D23" s="4" t="s">
+      <c r="H28" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="I28" s="51"/>
+      <c r="J28" s="51"/>
+      <c r="K28" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="L28" s="100"/>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D29" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E23" s="74"/>
-      <c r="F23" s="3" t="s">
+      <c r="E29" s="66"/>
+      <c r="F29" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="G29" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="13" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="24" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D24" s="4" t="s">
+      <c r="H29" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="I29" s="51"/>
+      <c r="J29" s="51"/>
+      <c r="K29" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="L29" s="100"/>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D30" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E24" s="74"/>
-      <c r="F24" s="3" t="s">
+      <c r="E30" s="66"/>
+      <c r="F30" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="G30" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="13" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="25" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D25" s="4" t="s">
+      <c r="H30" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="I30" s="51"/>
+      <c r="J30" s="51"/>
+      <c r="K30" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="L30" s="100"/>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D31" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E25" s="73"/>
-      <c r="F25" s="3" t="s">
+      <c r="E31" s="67"/>
+      <c r="F31" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G31" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
-      <c r="K25" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="N25" s="21"/>
-      <c r="O25" s="21"/>
-    </row>
-    <row r="26" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D26" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E26" s="66" t="s">
-        <v>62</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="N26" s="21"/>
-      <c r="O26" s="21">
-        <f>COUNTIF(K19:K102,"DangVH")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D27" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E27" s="67"/>
-      <c r="F27" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
-      <c r="K27" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="N27" s="21"/>
-      <c r="O27" s="21">
-        <f>COUNTIF(K20:K103,"HuyenPT")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D28" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E28" s="67"/>
-      <c r="F28" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="N28" s="21"/>
-      <c r="O28" s="21">
-        <f>COUNTIF(K21:K104,"VanTTC")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D29" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E29" s="68"/>
-      <c r="F29" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H29" s="22"/>
-      <c r="I29" s="22"/>
-      <c r="J29" s="22"/>
-      <c r="K29" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-    </row>
-    <row r="30" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D30" s="69" t="s">
-        <v>74</v>
-      </c>
-      <c r="E30" s="70"/>
-      <c r="F30" s="70"/>
-      <c r="G30" s="71"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="22"/>
-      <c r="J30" s="22"/>
-      <c r="K30" s="12"/>
-    </row>
-    <row r="31" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D31" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E31" s="66" t="s">
-        <v>76</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="H31" s="24" t="s">
-        <v>205</v>
-      </c>
-      <c r="I31" s="85">
-        <v>42593</v>
-      </c>
-      <c r="J31" s="24"/>
+      <c r="H31" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="I31" s="51"/>
+      <c r="J31" s="51"/>
       <c r="K31" s="15" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="32" spans="4:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="D32" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="E32" s="67"/>
-      <c r="F32" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="H32" s="25" t="s">
-        <v>209</v>
-      </c>
-      <c r="I32" s="47">
-        <v>42593</v>
-      </c>
-      <c r="J32" s="25"/>
-      <c r="K32" s="15" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="33" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D33" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="E33" s="68"/>
-      <c r="F33" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="H33" s="22"/>
-      <c r="I33" s="22"/>
-      <c r="J33" s="22"/>
-      <c r="K33" s="13" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="34" spans="4:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="D34" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="E34" s="72" t="s">
-        <v>86</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="H34" s="26" t="s">
-        <v>210</v>
-      </c>
-      <c r="I34" s="46">
-        <v>42593</v>
-      </c>
-      <c r="J34" s="26"/>
-      <c r="K34" s="15" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="35" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D35" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="E35" s="74"/>
-      <c r="F35" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="H35" s="22"/>
-      <c r="I35" s="22"/>
-      <c r="J35" s="22"/>
-      <c r="K35" s="13" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="36" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D36" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="E36" s="73"/>
-      <c r="F36" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>94</v>
-      </c>
+      <c r="L31" s="100"/>
+      <c r="M31" s="21"/>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D32" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" s="62" t="s">
+        <v>62</v>
+      </c>
+      <c r="F32" s="88" t="s">
+        <v>63</v>
+      </c>
+      <c r="G32" s="88" t="s">
+        <v>64</v>
+      </c>
+      <c r="H32" s="92"/>
+      <c r="I32" s="92"/>
+      <c r="J32" s="92"/>
+      <c r="K32" s="93"/>
+      <c r="L32" s="97"/>
+      <c r="M32" s="21">
+        <f>COUNTIF(K25:K108,"DangVH")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D33" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E33" s="63"/>
+      <c r="F33" s="88" t="s">
+        <v>66</v>
+      </c>
+      <c r="G33" s="88" t="s">
+        <v>67</v>
+      </c>
+      <c r="H33" s="92"/>
+      <c r="I33" s="92"/>
+      <c r="J33" s="92"/>
+      <c r="K33" s="93"/>
+      <c r="L33" s="97"/>
+      <c r="M33" s="21">
+        <f>COUNTIF(K26:K109,"HuyenPT")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D34" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E34" s="63"/>
+      <c r="F34" s="88" t="s">
+        <v>69</v>
+      </c>
+      <c r="G34" s="88" t="s">
+        <v>70</v>
+      </c>
+      <c r="H34" s="92"/>
+      <c r="I34" s="92"/>
+      <c r="J34" s="92"/>
+      <c r="K34" s="93"/>
+      <c r="L34" s="97"/>
+      <c r="M34" s="21">
+        <f>COUNTIF(K27:K110,"VanTTC")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D35" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E35" s="64"/>
+      <c r="F35" s="88" t="s">
+        <v>72</v>
+      </c>
+      <c r="G35" s="88" t="s">
+        <v>73</v>
+      </c>
+      <c r="H35" s="92"/>
+      <c r="I35" s="92"/>
+      <c r="J35" s="92"/>
+      <c r="K35" s="93"/>
+      <c r="L35" s="97"/>
+      <c r="M35" s="1"/>
+    </row>
+    <row r="36" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D36" s="80" t="s">
+        <v>74</v>
+      </c>
+      <c r="E36" s="81"/>
+      <c r="F36" s="81"/>
+      <c r="G36" s="82"/>
       <c r="H36" s="22"/>
       <c r="I36" s="22"/>
       <c r="J36" s="22"/>
-      <c r="K36" s="13" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="37" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D37" s="63" t="s">
-        <v>95</v>
-      </c>
-      <c r="E37" s="64"/>
-      <c r="F37" s="64"/>
-      <c r="G37" s="65"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="22"/>
-      <c r="J37" s="22"/>
-      <c r="K37" s="13" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="38" spans="4:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="D38" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E38" s="72" t="s">
-        <v>97</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>98</v>
+      <c r="K36" s="12"/>
+      <c r="L36" s="96"/>
+    </row>
+    <row r="37" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D37" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E37" s="62" t="s">
+        <v>76</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H37" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="I37" s="48">
+        <v>42593</v>
+      </c>
+      <c r="J37" s="24"/>
+      <c r="K37" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="L37" s="100"/>
+    </row>
+    <row r="38" spans="4:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="D38" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E38" s="63"/>
+      <c r="F38" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="H38" s="26" t="s">
-        <v>210</v>
-      </c>
-      <c r="I38" s="46">
-        <v>42411</v>
-      </c>
-      <c r="J38" s="46"/>
-      <c r="K38" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="L38" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="39" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D39" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E39" s="74"/>
-      <c r="F39" s="3" t="s">
-        <v>101</v>
+        <v>81</v>
+      </c>
+      <c r="H38" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="I38" s="47">
+        <v>42593</v>
+      </c>
+      <c r="J38" s="25"/>
+      <c r="K38" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="L38" s="100"/>
+    </row>
+    <row r="39" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D39" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E39" s="64"/>
+      <c r="F39" s="5" t="s">
+        <v>83</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="H39" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="I39" s="46">
-        <v>42411</v>
-      </c>
-      <c r="J39" s="46">
-        <v>42562</v>
-      </c>
-      <c r="K39" s="14" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="40" spans="4:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="D40" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E40" s="73"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="26"/>
+      <c r="K39" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="L39" s="100"/>
+    </row>
+    <row r="40" spans="4:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="D40" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="E40" s="65" t="s">
+        <v>86</v>
+      </c>
       <c r="F40" s="3" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="H40" s="26" t="s">
         <v>210</v>
       </c>
       <c r="I40" s="46">
-        <v>42411</v>
+        <v>42593</v>
       </c>
       <c r="J40" s="26"/>
-      <c r="K40" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="L40" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="41" spans="4:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="D41" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E41" s="66" t="s">
-        <v>107</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>109</v>
+      <c r="K40" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="L40" s="14" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="41" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D41" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E41" s="66"/>
+      <c r="F41" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="H41" s="26" t="s">
         <v>210</v>
       </c>
       <c r="I41" s="46">
-        <v>42411</v>
+        <v>42594</v>
       </c>
       <c r="J41" s="26"/>
-      <c r="K41" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="L41" s="84" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="42" spans="4:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="D42" s="4" t="s">
-        <v>113</v>
+      <c r="K41" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="L41" s="14" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="42" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D42" s="11" t="s">
+        <v>96</v>
       </c>
       <c r="E42" s="67"/>
-      <c r="F42" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="G42" s="6" t="s">
-        <v>112</v>
+      <c r="F42" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="H42" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="I42" s="46">
-        <v>42411</v>
-      </c>
+      <c r="I42" s="26"/>
       <c r="J42" s="26"/>
       <c r="K42" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="L42" s="1" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="43" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D43" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E43" s="67"/>
-      <c r="F43" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="H43" s="26" t="s">
-        <v>210</v>
-      </c>
-      <c r="I43" s="46">
-        <v>42411</v>
-      </c>
-      <c r="J43" s="46">
-        <v>42562</v>
-      </c>
-      <c r="K43" s="14" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="44" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="L42" s="100"/>
+    </row>
+    <row r="43" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D43" s="77" t="s">
+        <v>95</v>
+      </c>
+      <c r="E43" s="78"/>
+      <c r="F43" s="78"/>
+      <c r="G43" s="79"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
+      <c r="K43" s="27"/>
+      <c r="L43" s="96"/>
+    </row>
+    <row r="44" spans="4:13" ht="30" x14ac:dyDescent="0.25">
       <c r="D44" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="E44" s="68"/>
+        <v>100</v>
+      </c>
+      <c r="E44" s="65" t="s">
+        <v>97</v>
+      </c>
       <c r="F44" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>118</v>
+        <v>98</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>99</v>
       </c>
       <c r="H44" s="26" t="s">
         <v>210</v>
@@ -2515,683 +2556,899 @@
       <c r="I44" s="46">
         <v>42411</v>
       </c>
-      <c r="J44" s="46">
+      <c r="J44" s="46"/>
+      <c r="K44" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="L44" s="14" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="45" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D45" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E45" s="66"/>
+      <c r="F45" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="H45" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="I45" s="46">
+        <v>42411</v>
+      </c>
+      <c r="J45" s="46">
         <v>42562</v>
       </c>
-      <c r="K44" s="14" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="45" spans="4:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="D45" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E45" s="72" t="s">
-        <v>120</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G45" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="H45" s="22"/>
-      <c r="I45" s="22"/>
-      <c r="J45" s="22"/>
-      <c r="K45" s="13" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="46" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="K45" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="L45" s="14" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="46" spans="4:13" ht="45" x14ac:dyDescent="0.25">
       <c r="D46" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="E46" s="74"/>
-      <c r="F46" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H46" s="22"/>
-      <c r="I46" s="22"/>
-      <c r="J46" s="22"/>
-      <c r="K46" s="13" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="47" spans="4:12" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="E46" s="67"/>
+      <c r="F46" s="88" t="s">
+        <v>104</v>
+      </c>
+      <c r="G46" s="89" t="s">
+        <v>105</v>
+      </c>
+      <c r="H46" s="92"/>
+      <c r="I46" s="103"/>
+      <c r="J46" s="92"/>
+      <c r="K46" s="104"/>
+      <c r="L46" s="97"/>
+    </row>
+    <row r="47" spans="4:13" s="109" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="D47" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="E47" s="73"/>
-      <c r="F47" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="H47" s="22"/>
-      <c r="I47" s="22"/>
-      <c r="J47" s="22"/>
-      <c r="K47" s="13" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="48" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D48" s="63" t="s">
-        <v>129</v>
-      </c>
-      <c r="E48" s="64"/>
-      <c r="F48" s="64"/>
-      <c r="G48" s="65"/>
-      <c r="H48" s="22"/>
-      <c r="I48" s="22"/>
-      <c r="J48" s="22"/>
-      <c r="K48" s="12"/>
+        <v>110</v>
+      </c>
+      <c r="E47" s="62" t="s">
+        <v>107</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="H47" s="105" t="s">
+        <v>210</v>
+      </c>
+      <c r="I47" s="106">
+        <v>42411</v>
+      </c>
+      <c r="J47" s="105"/>
+      <c r="K47" s="107" t="s">
+        <v>207</v>
+      </c>
+      <c r="L47" s="108" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="48" spans="4:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="D48" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E48" s="63"/>
+      <c r="F48" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="H48" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="I48" s="46">
+        <v>42411</v>
+      </c>
+      <c r="J48" s="26"/>
+      <c r="K48" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="L48" s="98" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D49" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="E49" s="4"/>
+        <v>116</v>
+      </c>
+      <c r="E49" s="63"/>
       <c r="F49" s="3" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="H49" s="22"/>
-      <c r="I49" s="22"/>
-      <c r="J49" s="22"/>
-      <c r="K49" s="13" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="H49" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="I49" s="46">
+        <v>42411</v>
+      </c>
+      <c r="J49" s="46">
+        <v>42562</v>
+      </c>
+      <c r="K49" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="L49" s="98" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D50" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="E50" s="4"/>
-      <c r="F50" s="5" t="s">
-        <v>134</v>
+        <v>119</v>
+      </c>
+      <c r="E50" s="64"/>
+      <c r="F50" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="H50" s="22"/>
-      <c r="I50" s="22"/>
-      <c r="J50" s="22"/>
-      <c r="K50" s="13" t="s">
-        <v>208</v>
+        <v>118</v>
+      </c>
+      <c r="H50" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="I50" s="46">
+        <v>42411</v>
+      </c>
+      <c r="J50" s="46">
+        <v>42562</v>
+      </c>
+      <c r="K50" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="L50" s="98" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="D51" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="E51" s="4"/>
-      <c r="F51" s="3" t="s">
-        <v>200</v>
+        <v>123</v>
+      </c>
+      <c r="E51" s="65" t="s">
+        <v>120</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>121</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="H51" s="22"/>
-      <c r="I51" s="22"/>
-      <c r="J51" s="22"/>
-      <c r="K51" s="13" t="s">
-        <v>208</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="H51" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="I51" s="25"/>
+      <c r="J51" s="25"/>
+      <c r="K51" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="L51" s="100"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D52" s="62" t="s">
-        <v>136</v>
-      </c>
-      <c r="E52" s="62"/>
-      <c r="F52" s="62"/>
-      <c r="G52" s="62"/>
-      <c r="H52" s="22"/>
-      <c r="I52" s="22"/>
-      <c r="J52" s="22"/>
-      <c r="K52" s="12"/>
+      <c r="D52" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E52" s="66"/>
+      <c r="F52" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="H52" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="I52" s="25"/>
+      <c r="J52" s="25"/>
+      <c r="K52" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="L52" s="100"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D53" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="E53" s="59" t="s">
-        <v>138</v>
-      </c>
-      <c r="F53" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="G53" s="9"/>
-      <c r="H53" s="22"/>
-      <c r="I53" s="22"/>
-      <c r="J53" s="22"/>
-      <c r="K53" s="13" t="s">
-        <v>208</v>
-      </c>
+      <c r="D53" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E53" s="67"/>
+      <c r="F53" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="H53" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="I53" s="25"/>
+      <c r="J53" s="25"/>
+      <c r="K53" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="L53" s="100"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D54" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="E54" s="60"/>
-      <c r="F54" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="G54" s="9" t="s">
-        <v>142</v>
-      </c>
+      <c r="D54" s="77" t="s">
+        <v>129</v>
+      </c>
+      <c r="E54" s="78"/>
+      <c r="F54" s="78"/>
+      <c r="G54" s="79"/>
       <c r="H54" s="22"/>
       <c r="I54" s="22"/>
       <c r="J54" s="22"/>
-      <c r="K54" s="13" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D55" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="E55" s="60"/>
-      <c r="F55" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="G55" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="H55" s="22"/>
-      <c r="I55" s="22"/>
-      <c r="J55" s="22"/>
-      <c r="K55" s="13" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D56" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="E56" s="60"/>
-      <c r="F56" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="G56" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="H56" s="22"/>
-      <c r="I56" s="22"/>
-      <c r="J56" s="22"/>
+      <c r="K54" s="12"/>
+      <c r="L54" s="96"/>
+    </row>
+    <row r="55" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="D55" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E55" s="4"/>
+      <c r="F55" s="90" t="s">
+        <v>131</v>
+      </c>
+      <c r="G55" s="90" t="s">
+        <v>132</v>
+      </c>
+      <c r="H55" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="I55" s="46">
+        <v>42411</v>
+      </c>
+      <c r="J55" s="46">
+        <v>42562</v>
+      </c>
+      <c r="K55" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="L55" s="99" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="D56" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E56" s="4"/>
+      <c r="F56" s="91" t="s">
+        <v>134</v>
+      </c>
+      <c r="G56" s="90" t="s">
+        <v>135</v>
+      </c>
+      <c r="H56" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="I56" s="24"/>
+      <c r="J56" s="24"/>
       <c r="K56" s="13" t="s">
         <v>208</v>
       </c>
+      <c r="L56" s="114"/>
     </row>
     <row r="57" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>209</v>
-      </c>
-      <c r="D57" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="E57" s="60"/>
-      <c r="F57" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="G57" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="H57" s="22"/>
-      <c r="I57" s="22"/>
-      <c r="J57" s="22"/>
-      <c r="K57" s="13" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>210</v>
-      </c>
-      <c r="D58" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="E58" s="61"/>
-      <c r="F58" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="G58" s="10" t="s">
-        <v>154</v>
-      </c>
+      <c r="D57" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E57" s="4"/>
+      <c r="F57" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="H57" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="I57" s="24"/>
+      <c r="J57" s="24"/>
+      <c r="K57" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="L57" s="100" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D58" s="71" t="s">
+        <v>136</v>
+      </c>
+      <c r="E58" s="71"/>
+      <c r="F58" s="71"/>
+      <c r="G58" s="71"/>
       <c r="H58" s="22"/>
       <c r="I58" s="22"/>
       <c r="J58" s="22"/>
-      <c r="K58" s="13" t="s">
-        <v>208</v>
-      </c>
+      <c r="K58" s="12"/>
+      <c r="L58" s="96"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>205</v>
-      </c>
       <c r="D59" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="E59" s="59" t="s">
-        <v>156</v>
+        <v>143</v>
+      </c>
+      <c r="E59" s="68" t="s">
+        <v>138</v>
       </c>
       <c r="F59" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="G59" s="9" t="s">
-        <v>158</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="G59" s="9"/>
       <c r="H59" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="I59" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="J59" s="26" t="s">
-        <v>237</v>
-      </c>
-      <c r="K59" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="L59" s="88" t="s">
-        <v>246</v>
-      </c>
+      <c r="I59" s="110"/>
+      <c r="J59" s="110"/>
+      <c r="K59" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="L59" s="114"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D60" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="E60" s="60"/>
+        <v>146</v>
+      </c>
+      <c r="E60" s="69"/>
       <c r="F60" s="9" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G60" s="9" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="H60" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="I60" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="J60" s="26" t="s">
-        <v>237</v>
-      </c>
-      <c r="K60" s="14" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="I60" s="110"/>
+      <c r="J60" s="110"/>
+      <c r="K60" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="L60" s="114"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D61" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="E61" s="61"/>
-      <c r="F61" s="10" t="s">
-        <v>163</v>
+        <v>149</v>
+      </c>
+      <c r="E61" s="69"/>
+      <c r="F61" s="9" t="s">
+        <v>144</v>
       </c>
       <c r="G61" s="9" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="H61" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="I61" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="J61" s="26" t="s">
-        <v>237</v>
-      </c>
+      <c r="I61" s="110"/>
+      <c r="J61" s="110"/>
       <c r="K61" s="13" t="s">
         <v>208</v>
       </c>
+      <c r="L61" s="114"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D62" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="E62" s="59" t="s">
-        <v>166</v>
-      </c>
-      <c r="F62" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="G62" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="H62" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="E62" s="69"/>
+      <c r="F62" s="88" t="s">
+        <v>147</v>
+      </c>
+      <c r="G62" s="88" t="s">
+        <v>148</v>
+      </c>
+      <c r="H62" s="92"/>
+      <c r="I62" s="92"/>
+      <c r="J62" s="92"/>
+      <c r="K62" s="93"/>
+      <c r="L62" s="97"/>
+    </row>
+    <row r="63" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>209</v>
       </c>
-      <c r="I62" s="25" t="s">
-        <v>238</v>
-      </c>
-      <c r="J62" s="25" t="s">
-        <v>238</v>
-      </c>
-      <c r="K62" s="14" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D63" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="E63" s="60"/>
-      <c r="F63" s="9" t="s">
-        <v>170</v>
+        <v>155</v>
+      </c>
+      <c r="E63" s="69"/>
+      <c r="F63" s="10" t="s">
+        <v>150</v>
       </c>
       <c r="G63" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="H63" s="25" t="s">
-        <v>209</v>
-      </c>
-      <c r="I63" s="25" t="s">
-        <v>239</v>
-      </c>
-      <c r="J63" s="25" t="s">
-        <v>239</v>
-      </c>
-      <c r="K63" s="14" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="H63" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="I63" s="110"/>
+      <c r="J63" s="110"/>
+      <c r="K63" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="L63" s="114"/>
+    </row>
+    <row r="64" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>210</v>
+      </c>
       <c r="D64" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="E64" s="60"/>
-      <c r="F64" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="G64" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="H64" s="25" t="s">
-        <v>209</v>
-      </c>
-      <c r="I64" s="25"/>
-      <c r="J64" s="25"/>
+        <v>159</v>
+      </c>
+      <c r="E64" s="70"/>
+      <c r="F64" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="G64" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="H64" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="I64" s="110"/>
+      <c r="J64" s="110"/>
       <c r="K64" s="13" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="65" spans="4:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L64" s="114"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>205</v>
+      </c>
       <c r="D65" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="E65" s="60"/>
+        <v>162</v>
+      </c>
+      <c r="E65" s="68" t="s">
+        <v>156</v>
+      </c>
       <c r="F65" s="9" t="s">
-        <v>213</v>
+        <v>157</v>
       </c>
       <c r="G65" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="H65" s="25" t="s">
-        <v>209</v>
-      </c>
-      <c r="I65" s="25"/>
-      <c r="J65" s="25"/>
-      <c r="K65" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="H65" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="I65" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="J65" s="26" t="s">
+        <v>237</v>
+      </c>
+      <c r="K65" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="L65" s="14" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D66" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="E66" s="69"/>
+      <c r="F66" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="G66" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H66" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="I66" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="J66" s="26" t="s">
+        <v>237</v>
+      </c>
+      <c r="K66" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="L66" s="14" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="D67" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="E67" s="70"/>
+      <c r="F67" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="G67" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="H67" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="I67" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="J67" s="26" t="s">
+        <v>237</v>
+      </c>
+      <c r="K67" s="13" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="66" spans="4:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D66" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="E66" s="61"/>
-      <c r="F66" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="G66" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="H66" s="25" t="s">
-        <v>209</v>
-      </c>
-      <c r="I66" s="25"/>
-      <c r="J66" s="25"/>
-      <c r="K66" s="13" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="67" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D67" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="E67" s="59" t="s">
-        <v>176</v>
-      </c>
-      <c r="F67" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="G67" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="H67" s="25" t="s">
-        <v>209</v>
-      </c>
-      <c r="I67" s="47">
-        <v>42380</v>
-      </c>
-      <c r="J67" s="47">
-        <v>42411</v>
-      </c>
-      <c r="K67" s="14" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="68" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L67" s="114"/>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D68" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="E68" s="60"/>
+        <v>172</v>
+      </c>
+      <c r="E68" s="68" t="s">
+        <v>166</v>
+      </c>
       <c r="F68" s="9" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="G68" s="9" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="H68" s="25" t="s">
         <v>209</v>
       </c>
-      <c r="I68" s="47">
-        <v>42380</v>
-      </c>
-      <c r="J68" s="47"/>
-      <c r="K68" s="15" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="69" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="I68" s="25" t="s">
+        <v>238</v>
+      </c>
+      <c r="J68" s="25" t="s">
+        <v>238</v>
+      </c>
+      <c r="K68" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="L68" s="98"/>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D69" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="E69" s="61"/>
+        <v>175</v>
+      </c>
+      <c r="E69" s="69"/>
       <c r="F69" s="9" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="G69" s="9" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="H69" s="25" t="s">
         <v>209</v>
       </c>
-      <c r="I69" s="47">
+      <c r="I69" s="25" t="s">
+        <v>239</v>
+      </c>
+      <c r="J69" s="25" t="s">
+        <v>239</v>
+      </c>
+      <c r="K69" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="L69" s="98"/>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D70" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="E70" s="69"/>
+      <c r="F70" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="G70" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="H70" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="I70" s="25"/>
+      <c r="J70" s="25"/>
+      <c r="K70" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="L70" s="98"/>
+    </row>
+    <row r="71" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D71" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="E71" s="69"/>
+      <c r="F71" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="G71" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="H71" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="I71" s="25"/>
+      <c r="J71" s="25"/>
+      <c r="K71" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="L71" s="98"/>
+    </row>
+    <row r="72" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D72" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="E72" s="70"/>
+      <c r="F72" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="G72" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="H72" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="I72" s="25"/>
+      <c r="J72" s="25"/>
+      <c r="K72" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="L72" s="98"/>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D73" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="E73" s="68" t="s">
+        <v>176</v>
+      </c>
+      <c r="F73" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="G73" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="H73" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="I73" s="47">
         <v>42380</v>
       </c>
-      <c r="J69" s="47">
+      <c r="J73" s="47">
         <v>42411</v>
       </c>
-      <c r="K69" s="14" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="70" spans="4:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="D70" s="59" t="s">
+      <c r="K73" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="L73" s="98"/>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D74" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="E74" s="69"/>
+      <c r="F74" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="G74" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="H74" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="I74" s="47">
+        <v>42380</v>
+      </c>
+      <c r="J74" s="47"/>
+      <c r="K74" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="L74" s="98"/>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D75" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="E75" s="70"/>
+      <c r="F75" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="G75" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="H75" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="I75" s="47">
+        <v>42380</v>
+      </c>
+      <c r="J75" s="47">
+        <v>42411</v>
+      </c>
+      <c r="K75" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="L75" s="98"/>
+    </row>
+    <row r="76" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="D76" s="68" t="s">
         <v>217</v>
       </c>
-      <c r="E70" s="59" t="s">
+      <c r="E76" s="68" t="s">
         <v>186</v>
       </c>
-      <c r="F70" s="10" t="s">
+      <c r="F76" s="91" t="s">
         <v>187</v>
       </c>
-      <c r="G70" s="10" t="s">
+      <c r="G76" s="91" t="s">
         <v>188</v>
       </c>
-      <c r="H70" s="52"/>
-      <c r="I70" s="52"/>
-      <c r="J70" s="52"/>
-      <c r="K70" s="49" t="s">
+      <c r="H76" s="111" t="s">
+        <v>210</v>
+      </c>
+      <c r="I76" s="111"/>
+      <c r="J76" s="111"/>
+      <c r="K76" s="53" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="71" spans="4:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="D71" s="60"/>
-      <c r="E71" s="60"/>
-      <c r="F71" s="10" t="s">
+      <c r="L76" s="115"/>
+    </row>
+    <row r="77" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="D77" s="69"/>
+      <c r="E77" s="69"/>
+      <c r="F77" s="91" t="s">
         <v>189</v>
       </c>
-      <c r="G71" s="10" t="s">
+      <c r="G77" s="91" t="s">
         <v>190</v>
       </c>
-      <c r="H71" s="53"/>
-      <c r="I71" s="53"/>
-      <c r="J71" s="53"/>
-      <c r="K71" s="50"/>
-    </row>
-    <row r="72" spans="4:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="D72" s="60"/>
-      <c r="E72" s="60"/>
-      <c r="F72" s="10" t="s">
+      <c r="H77" s="112"/>
+      <c r="I77" s="112"/>
+      <c r="J77" s="112"/>
+      <c r="K77" s="54"/>
+      <c r="L77" s="115"/>
+    </row>
+    <row r="78" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="D78" s="69"/>
+      <c r="E78" s="69"/>
+      <c r="F78" s="91" t="s">
         <v>191</v>
       </c>
-      <c r="G72" s="10" t="s">
+      <c r="G78" s="91" t="s">
         <v>192</v>
       </c>
-      <c r="H72" s="53"/>
-      <c r="I72" s="53"/>
-      <c r="J72" s="53"/>
-      <c r="K72" s="50"/>
-    </row>
-    <row r="73" spans="4:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="D73" s="60"/>
-      <c r="E73" s="60"/>
-      <c r="F73" s="10" t="s">
+      <c r="H78" s="112"/>
+      <c r="I78" s="112"/>
+      <c r="J78" s="112"/>
+      <c r="K78" s="54"/>
+      <c r="L78" s="115"/>
+    </row>
+    <row r="79" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="D79" s="69"/>
+      <c r="E79" s="69"/>
+      <c r="F79" s="91" t="s">
         <v>193</v>
       </c>
-      <c r="G73" s="10" t="s">
+      <c r="G79" s="91" t="s">
         <v>194</v>
       </c>
-      <c r="H73" s="53"/>
-      <c r="I73" s="53"/>
-      <c r="J73" s="53"/>
-      <c r="K73" s="50"/>
-    </row>
-    <row r="74" spans="4:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="D74" s="61"/>
-      <c r="E74" s="61"/>
-      <c r="F74" s="10" t="s">
+      <c r="H79" s="112"/>
+      <c r="I79" s="112"/>
+      <c r="J79" s="112"/>
+      <c r="K79" s="54"/>
+      <c r="L79" s="115"/>
+    </row>
+    <row r="80" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="D80" s="70"/>
+      <c r="E80" s="70"/>
+      <c r="F80" s="91" t="s">
         <v>195</v>
       </c>
-      <c r="G74" s="9" t="s">
+      <c r="G80" s="90" t="s">
         <v>196</v>
       </c>
-      <c r="H74" s="54"/>
-      <c r="I74" s="54"/>
-      <c r="J74" s="54"/>
-      <c r="K74" s="51"/>
-    </row>
-    <row r="75" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D75" s="8" t="s">
+      <c r="H80" s="113"/>
+      <c r="I80" s="113"/>
+      <c r="J80" s="113"/>
+      <c r="K80" s="55"/>
+      <c r="L80" s="115"/>
+    </row>
+    <row r="81" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D81" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="E81" s="72" t="s">
+        <v>251</v>
+      </c>
+      <c r="F81" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="G81" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="H81" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="I81" s="46"/>
+      <c r="J81" s="46">
+        <v>42562</v>
+      </c>
+      <c r="K81" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="L81" s="98"/>
+    </row>
+    <row r="82" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D82" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="E82" s="72"/>
+      <c r="F82" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="E75" s="86" t="s">
-        <v>254</v>
-      </c>
-      <c r="F75" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="G75" s="10" t="s">
+      <c r="G82" s="10" t="s">
         <v>247</v>
       </c>
-      <c r="H75" s="26" t="s">
+      <c r="H82" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="I75" s="46"/>
-      <c r="J75" s="46">
+      <c r="I82" s="46"/>
+      <c r="J82" s="46">
         <v>42562</v>
       </c>
-      <c r="K75" s="14" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="76" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D76" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="E76" s="86"/>
-      <c r="F76" s="10" t="s">
-        <v>258</v>
-      </c>
-      <c r="G76" s="10" t="s">
-        <v>248</v>
-      </c>
-      <c r="H76" s="26" t="s">
-        <v>210</v>
-      </c>
-      <c r="I76" s="46"/>
-      <c r="J76" s="46">
-        <v>42562</v>
-      </c>
-      <c r="K76" s="14" t="s">
-        <v>206</v>
-      </c>
+      <c r="K82" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="L82" s="98"/>
     </row>
   </sheetData>
-  <autoFilter ref="K4:K84"/>
-  <mergeCells count="33">
-    <mergeCell ref="E75:E76"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="D48:G48"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="D30:G30"/>
-    <mergeCell ref="D37:G37"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E16:E21"/>
-    <mergeCell ref="E22:E25"/>
-    <mergeCell ref="E31:E33"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="E41:E44"/>
-    <mergeCell ref="E38:E40"/>
-    <mergeCell ref="E45:E47"/>
-    <mergeCell ref="E67:E69"/>
-    <mergeCell ref="E70:E74"/>
-    <mergeCell ref="D52:G52"/>
-    <mergeCell ref="E53:E58"/>
-    <mergeCell ref="D70:D74"/>
-    <mergeCell ref="E62:E66"/>
-    <mergeCell ref="E59:E61"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="K70:K74"/>
-    <mergeCell ref="H70:H74"/>
-    <mergeCell ref="I70:I74"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="J70:J74"/>
+  <autoFilter ref="H10:H82"/>
+  <mergeCells count="35">
+    <mergeCell ref="E81:E82"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="E13:E16"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="D54:G54"/>
+    <mergeCell ref="E32:E35"/>
+    <mergeCell ref="D36:G36"/>
+    <mergeCell ref="D43:G43"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E22:E27"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="E37:E39"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="E47:E50"/>
+    <mergeCell ref="E44:E46"/>
+    <mergeCell ref="E51:E53"/>
+    <mergeCell ref="E73:E75"/>
+    <mergeCell ref="E76:E80"/>
+    <mergeCell ref="D58:G58"/>
+    <mergeCell ref="E59:E64"/>
+    <mergeCell ref="D76:D80"/>
+    <mergeCell ref="E68:E72"/>
+    <mergeCell ref="E65:E67"/>
+    <mergeCell ref="K76:K80"/>
+    <mergeCell ref="H76:H80"/>
+    <mergeCell ref="I76:I80"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="K23:K24"/>
+    <mergeCell ref="J76:J80"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="L76:L80"/>
+    <mergeCell ref="L23:L24"/>
   </mergeCells>
-  <conditionalFormatting sqref="M7:N9">
+  <conditionalFormatting sqref="H3:I5">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -3204,14 +3461,14 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B9 H38:H47 H7:H14 H16:H17 H19:H29 H31:H36">
-      <formula1>$B$7:$B$9</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15 H55 H13:H20 H22:H23 H44:H53 H37:H42 H25:H35">
+      <formula1>$B$13:$B$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H49:H51 H53:H70 H75:H76">
-      <formula1>$A$57:$A$59</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H81:H82 H56:H57 H59:H76">
+      <formula1>$A$63:$A$65</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M7:M9 K7:K17 K75:K76 K19:K70">
-      <formula1>$B$12:$B$14</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L65:L66 H3:H5 K13:K23 K81:K82 L48:L50 K25:K76 L40:L41 L44:L45">
+      <formula1>$B$18:$B$20</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3259,16 +3516,16 @@
       <c r="I4" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="K4" s="48" t="s">
+      <c r="K4" s="52" t="s">
         <v>215</v>
       </c>
-      <c r="L4" s="48"/>
+      <c r="L4" s="52"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="D5" s="59" t="s">
+      <c r="D5" s="68" t="s">
         <v>231</v>
       </c>
       <c r="E5" s="9" t="s">
@@ -3298,7 +3555,7 @@
       <c r="B6" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="D6" s="60"/>
+      <c r="D6" s="69"/>
       <c r="E6" s="9" t="s">
         <v>233</v>
       </c>
@@ -3322,7 +3579,7 @@
       <c r="B7" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="D7" s="79" t="s">
+      <c r="D7" s="83" t="s">
         <v>222</v>
       </c>
       <c r="E7" s="33" t="s">
@@ -3348,7 +3605,7 @@
       <c r="B8" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="D8" s="80"/>
+      <c r="D8" s="84"/>
       <c r="E8" s="33" t="s">
         <v>225</v>
       </c>
@@ -3364,7 +3621,7 @@
       <c r="L8" s="39"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D9" s="81"/>
+      <c r="D9" s="85"/>
       <c r="E9" s="33" t="s">
         <v>226</v>
       </c>
@@ -3380,7 +3637,7 @@
       <c r="L9" s="39"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D10" s="82" t="s">
+      <c r="D10" s="86" t="s">
         <v>227</v>
       </c>
       <c r="E10" s="34" t="s">
@@ -3401,7 +3658,7 @@
       <c r="B11" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="D11" s="83"/>
+      <c r="D11" s="87"/>
       <c r="E11" s="34" t="s">
         <v>234</v>
       </c>
@@ -3518,10 +3775,10 @@
       <c r="H4" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="J4" s="48" t="s">
+      <c r="J4" s="52" t="s">
         <v>215</v>
       </c>
-      <c r="K4" s="48"/>
+      <c r="K4" s="52"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -3578,14 +3835,14 @@
         <v>207</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E7" s="23" t="s">
         <v>221</v>
       </c>
       <c r="F7" s="30"/>
       <c r="G7" s="30" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="H7" s="27"/>
       <c r="J7" s="21" t="s">
@@ -3615,7 +3872,7 @@
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="F14" s="19" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Doc]_Update các task của dự án
</commit_message>
<xml_diff>
--- a/WIP/Users/HuyenPT/Tiến độ các task  của dự án.xlsx
+++ b/WIP/Users/HuyenPT/Tiến độ các task  của dự án.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="268">
   <si>
     <t>Use Case No.</t>
   </si>
@@ -825,6 +825,9 @@
   </si>
   <si>
     <t>các phần có làm</t>
+  </si>
+  <si>
+    <t>Note:</t>
   </si>
 </sst>
 </file>
@@ -1095,7 +1098,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1212,114 +1215,6 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="11" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1357,12 +1252,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1385,24 +1274,139 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="11" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1722,17 +1726,22 @@
     <col min="7" max="7" width="50.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="15.5703125" style="19" customWidth="1"/>
     <col min="11" max="11" width="12.42578125" customWidth="1"/>
-    <col min="12" max="12" width="16.140625" style="94" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" style="58" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H1" s="19"/>
       <c r="I1" s="19"/>
       <c r="J1" s="19"/>
-      <c r="L1" s="94"/>
+      <c r="L1" s="58"/>
+    </row>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C2" s="77" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="3" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E3" s="116" t="s">
+      <c r="E3" s="74" t="s">
         <v>262</v>
       </c>
       <c r="F3" s="13" t="s">
@@ -1743,13 +1752,13 @@
       </c>
       <c r="I3" s="50">
         <f>COUNTIF(K13:K83,"Done")</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J3" s="19"/>
-      <c r="L3" s="94"/>
+      <c r="L3" s="58"/>
     </row>
     <row r="4" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E4" s="117" t="s">
+      <c r="E4" s="75" t="s">
         <v>263</v>
       </c>
       <c r="F4" s="15" t="s">
@@ -1763,10 +1772,10 @@
         <v>18</v>
       </c>
       <c r="J4" s="19"/>
-      <c r="L4" s="94"/>
+      <c r="L4" s="58"/>
     </row>
     <row r="5" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E5" s="118" t="s">
+      <c r="E5" s="76" t="s">
         <v>265</v>
       </c>
       <c r="F5" s="14" t="s">
@@ -1777,10 +1786,10 @@
       </c>
       <c r="I5" s="12">
         <f>COUNTIF(K13:K82, "Not Start")</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J5" s="19"/>
-      <c r="L5" s="94"/>
+      <c r="L5" s="58"/>
     </row>
     <row r="6" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H6" s="12" t="s">
@@ -1791,13 +1800,13 @@
         <v>52</v>
       </c>
       <c r="J6" s="19"/>
-      <c r="L6" s="94"/>
+      <c r="L6" s="58"/>
     </row>
     <row r="7" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
       <c r="J7" s="19"/>
-      <c r="L7" s="94"/>
+      <c r="L7" s="58"/>
     </row>
     <row r="10" spans="2:12" ht="42.75" x14ac:dyDescent="0.25">
       <c r="D10" s="2" t="s">
@@ -1824,82 +1833,82 @@
       <c r="K10" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="L10" s="95" t="s">
+      <c r="L10" s="59" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D11" s="71" t="s">
+      <c r="D11" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="71"/>
-      <c r="F11" s="71"/>
-      <c r="G11" s="71"/>
+      <c r="E11" s="79"/>
+      <c r="F11" s="79"/>
+      <c r="G11" s="79"/>
       <c r="H11" s="22"/>
       <c r="I11" s="22"/>
       <c r="J11" s="22"/>
       <c r="K11" s="12"/>
-      <c r="L11" s="96"/>
+      <c r="L11" s="60"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D12" s="73" t="s">
+      <c r="D12" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="73"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="73"/>
+      <c r="E12" s="80"/>
+      <c r="F12" s="80"/>
+      <c r="G12" s="80"/>
       <c r="H12" s="22"/>
       <c r="I12" s="22"/>
       <c r="J12" s="22"/>
       <c r="K12" s="12"/>
-      <c r="L12" s="96"/>
+      <c r="L12" s="60"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>209</v>
       </c>
-      <c r="D13" s="65" t="s">
+      <c r="D13" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="65" t="s">
+      <c r="E13" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="88" t="s">
+      <c r="F13" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="88" t="s">
+      <c r="G13" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="92"/>
-      <c r="I13" s="92"/>
-      <c r="J13" s="92"/>
-      <c r="K13" s="93"/>
-      <c r="L13" s="97"/>
+      <c r="H13" s="56"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="57"/>
+      <c r="L13" s="61"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>210</v>
       </c>
-      <c r="D14" s="66"/>
-      <c r="E14" s="66"/>
-      <c r="F14" s="88" t="s">
+      <c r="D14" s="82"/>
+      <c r="E14" s="82"/>
+      <c r="F14" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="88" t="s">
+      <c r="G14" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="92"/>
-      <c r="I14" s="92"/>
-      <c r="J14" s="92"/>
-      <c r="K14" s="93"/>
-      <c r="L14" s="97"/>
+      <c r="H14" s="56"/>
+      <c r="I14" s="56"/>
+      <c r="J14" s="56"/>
+      <c r="K14" s="57"/>
+      <c r="L14" s="61"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>205</v>
       </c>
-      <c r="D15" s="67"/>
-      <c r="E15" s="66"/>
+      <c r="D15" s="83"/>
+      <c r="E15" s="82"/>
       <c r="F15" s="3" t="s">
         <v>12</v>
       </c>
@@ -1918,7 +1927,7 @@
       <c r="K15" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="L15" s="98" t="s">
+      <c r="L15" s="62" t="s">
         <v>206</v>
       </c>
     </row>
@@ -1926,7 +1935,7 @@
       <c r="D16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="67"/>
+      <c r="E16" s="83"/>
       <c r="F16" s="3" t="s">
         <v>15</v>
       </c>
@@ -1945,7 +1954,7 @@
       <c r="K16" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="L16" s="99" t="s">
+      <c r="L16" s="63" t="s">
         <v>257</v>
       </c>
     </row>
@@ -1953,7 +1962,7 @@
       <c r="D17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="65" t="s">
+      <c r="E17" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F17" s="3" t="s">
@@ -1974,7 +1983,7 @@
       <c r="K17" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="L17" s="98" t="s">
+      <c r="L17" s="62" t="s">
         <v>206</v>
       </c>
     </row>
@@ -1985,7 +1994,7 @@
       <c r="D18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="67"/>
+      <c r="E18" s="83"/>
       <c r="F18" s="3" t="s">
         <v>21</v>
       </c>
@@ -2004,7 +2013,7 @@
       <c r="K18" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="L18" s="98" t="s">
+      <c r="L18" s="62" t="s">
         <v>206</v>
       </c>
     </row>
@@ -2032,7 +2041,7 @@
       <c r="K19" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="L19" s="100"/>
+      <c r="L19" s="64"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="17" t="s">
@@ -2056,34 +2065,34 @@
       <c r="K20" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="L20" s="98" t="s">
+      <c r="L20" s="62" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D21" s="74" t="s">
+      <c r="D21" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="75"/>
-      <c r="F21" s="75"/>
-      <c r="G21" s="76"/>
+      <c r="E21" s="85"/>
+      <c r="F21" s="85"/>
+      <c r="G21" s="86"/>
       <c r="H21" s="22"/>
       <c r="I21" s="22"/>
       <c r="J21" s="22"/>
       <c r="K21" s="12"/>
-      <c r="L21" s="96"/>
+      <c r="L21" s="60"/>
     </row>
     <row r="22" spans="2:13" ht="45" x14ac:dyDescent="0.25">
       <c r="D22" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E22" s="65" t="s">
+      <c r="E22" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="90" t="s">
+      <c r="F22" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="G22" s="91" t="s">
+      <c r="G22" s="55" t="s">
         <v>33</v>
       </c>
       <c r="H22" s="25" t="s">
@@ -2096,55 +2105,55 @@
       <c r="K22" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="L22" s="98" t="s">
+      <c r="L22" s="62" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D23" s="65" t="s">
+      <c r="D23" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="E23" s="66"/>
-      <c r="F23" s="90" t="s">
+      <c r="E23" s="82"/>
+      <c r="F23" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="G23" s="90" t="s">
+      <c r="G23" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="H23" s="56" t="s">
+      <c r="H23" s="108" t="s">
         <v>209</v>
       </c>
-      <c r="I23" s="60"/>
+      <c r="I23" s="112"/>
       <c r="J23" s="28"/>
-      <c r="K23" s="58" t="s">
+      <c r="K23" s="110" t="s">
         <v>207</v>
       </c>
-      <c r="L23" s="101"/>
+      <c r="L23" s="100"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D24" s="67"/>
-      <c r="E24" s="66"/>
-      <c r="F24" s="90" t="s">
+      <c r="D24" s="83"/>
+      <c r="E24" s="82"/>
+      <c r="F24" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="G24" s="90" t="s">
+      <c r="G24" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="H24" s="57"/>
-      <c r="I24" s="61"/>
+      <c r="H24" s="109"/>
+      <c r="I24" s="113"/>
       <c r="J24" s="29"/>
-      <c r="K24" s="59"/>
-      <c r="L24" s="102"/>
+      <c r="K24" s="111"/>
+      <c r="L24" s="101"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D25" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="66"/>
-      <c r="F25" s="90" t="s">
+      <c r="E25" s="82"/>
+      <c r="F25" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="G25" s="90" t="s">
+      <c r="G25" s="54" t="s">
         <v>41</v>
       </c>
       <c r="H25" s="25" t="s">
@@ -2155,17 +2164,17 @@
       <c r="K25" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="L25" s="100"/>
+      <c r="L25" s="64"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D26" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E26" s="66"/>
-      <c r="F26" s="90" t="s">
+      <c r="E26" s="82"/>
+      <c r="F26" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="G26" s="90" t="s">
+      <c r="G26" s="54" t="s">
         <v>44</v>
       </c>
       <c r="H26" s="25" t="s">
@@ -2176,17 +2185,17 @@
       <c r="K26" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="L26" s="100"/>
+      <c r="L26" s="64"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D27" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E27" s="67"/>
-      <c r="F27" s="90" t="s">
+      <c r="E27" s="83"/>
+      <c r="F27" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="G27" s="90" t="s">
+      <c r="G27" s="54" t="s">
         <v>47</v>
       </c>
       <c r="H27" s="25" t="s">
@@ -2197,13 +2206,13 @@
       <c r="K27" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="L27" s="100"/>
+      <c r="L27" s="64"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D28" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E28" s="65" t="s">
+      <c r="E28" s="81" t="s">
         <v>49</v>
       </c>
       <c r="F28" s="3" t="s">
@@ -2220,13 +2229,13 @@
       <c r="K28" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="L28" s="100"/>
+      <c r="L28" s="64"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D29" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E29" s="66"/>
+      <c r="E29" s="82"/>
       <c r="F29" s="3" t="s">
         <v>53</v>
       </c>
@@ -2241,13 +2250,13 @@
       <c r="K29" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="L29" s="100"/>
+      <c r="L29" s="64"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D30" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E30" s="66"/>
+      <c r="E30" s="82"/>
       <c r="F30" s="3" t="s">
         <v>56</v>
       </c>
@@ -2262,13 +2271,13 @@
       <c r="K30" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="L30" s="100"/>
+      <c r="L30" s="64"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D31" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E31" s="67"/>
+      <c r="E31" s="83"/>
       <c r="F31" s="3" t="s">
         <v>59</v>
       </c>
@@ -2283,27 +2292,27 @@
       <c r="K31" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="L31" s="100"/>
+      <c r="L31" s="64"/>
       <c r="M31" s="21"/>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D32" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E32" s="62" t="s">
+      <c r="E32" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="F32" s="88" t="s">
+      <c r="F32" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="G32" s="88" t="s">
+      <c r="G32" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="H32" s="92"/>
-      <c r="I32" s="92"/>
-      <c r="J32" s="92"/>
-      <c r="K32" s="93"/>
-      <c r="L32" s="97"/>
+      <c r="H32" s="56"/>
+      <c r="I32" s="56"/>
+      <c r="J32" s="56"/>
+      <c r="K32" s="57"/>
+      <c r="L32" s="61"/>
       <c r="M32" s="21">
         <f>COUNTIF(K25:K108,"DangVH")</f>
         <v>0</v>
@@ -2313,18 +2322,18 @@
       <c r="D33" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E33" s="63"/>
-      <c r="F33" s="88" t="s">
+      <c r="E33" s="91"/>
+      <c r="F33" s="52" t="s">
         <v>66</v>
       </c>
-      <c r="G33" s="88" t="s">
+      <c r="G33" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="H33" s="92"/>
-      <c r="I33" s="92"/>
-      <c r="J33" s="92"/>
-      <c r="K33" s="93"/>
-      <c r="L33" s="97"/>
+      <c r="H33" s="56"/>
+      <c r="I33" s="56"/>
+      <c r="J33" s="56"/>
+      <c r="K33" s="57"/>
+      <c r="L33" s="61"/>
       <c r="M33" s="21">
         <f>COUNTIF(K26:K109,"HuyenPT")</f>
         <v>0</v>
@@ -2334,18 +2343,18 @@
       <c r="D34" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E34" s="63"/>
-      <c r="F34" s="88" t="s">
+      <c r="E34" s="91"/>
+      <c r="F34" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="G34" s="88" t="s">
+      <c r="G34" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="H34" s="92"/>
-      <c r="I34" s="92"/>
-      <c r="J34" s="92"/>
-      <c r="K34" s="93"/>
-      <c r="L34" s="97"/>
+      <c r="H34" s="56"/>
+      <c r="I34" s="56"/>
+      <c r="J34" s="56"/>
+      <c r="K34" s="57"/>
+      <c r="L34" s="61"/>
       <c r="M34" s="21">
         <f>COUNTIF(K27:K110,"VanTTC")</f>
         <v>0</v>
@@ -2355,38 +2364,38 @@
       <c r="D35" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E35" s="64"/>
-      <c r="F35" s="88" t="s">
+      <c r="E35" s="92"/>
+      <c r="F35" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="G35" s="88" t="s">
+      <c r="G35" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="H35" s="92"/>
-      <c r="I35" s="92"/>
-      <c r="J35" s="92"/>
-      <c r="K35" s="93"/>
-      <c r="L35" s="97"/>
+      <c r="H35" s="56"/>
+      <c r="I35" s="56"/>
+      <c r="J35" s="56"/>
+      <c r="K35" s="57"/>
+      <c r="L35" s="61"/>
       <c r="M35" s="1"/>
     </row>
     <row r="36" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D36" s="80" t="s">
+      <c r="D36" s="93" t="s">
         <v>74</v>
       </c>
-      <c r="E36" s="81"/>
-      <c r="F36" s="81"/>
-      <c r="G36" s="82"/>
+      <c r="E36" s="94"/>
+      <c r="F36" s="94"/>
+      <c r="G36" s="95"/>
       <c r="H36" s="22"/>
       <c r="I36" s="22"/>
       <c r="J36" s="22"/>
       <c r="K36" s="12"/>
-      <c r="L36" s="96"/>
+      <c r="L36" s="60"/>
     </row>
     <row r="37" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D37" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E37" s="62" t="s">
+      <c r="E37" s="90" t="s">
         <v>76</v>
       </c>
       <c r="F37" s="3" t="s">
@@ -2405,13 +2414,13 @@
       <c r="K37" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="L37" s="100"/>
+      <c r="L37" s="64"/>
     </row>
     <row r="38" spans="4:13" ht="30" x14ac:dyDescent="0.25">
       <c r="D38" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="E38" s="63"/>
+      <c r="E38" s="91"/>
       <c r="F38" s="5" t="s">
         <v>80</v>
       </c>
@@ -2428,13 +2437,13 @@
       <c r="K38" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="L38" s="100"/>
+      <c r="L38" s="64"/>
     </row>
     <row r="39" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D39" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E39" s="64"/>
+      <c r="E39" s="92"/>
       <c r="F39" s="5" t="s">
         <v>83</v>
       </c>
@@ -2449,13 +2458,13 @@
       <c r="K39" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="L39" s="100"/>
+      <c r="L39" s="64"/>
     </row>
     <row r="40" spans="4:13" ht="45" x14ac:dyDescent="0.25">
       <c r="D40" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="E40" s="65" t="s">
+      <c r="E40" s="81" t="s">
         <v>86</v>
       </c>
       <c r="F40" s="3" t="s">
@@ -2482,7 +2491,7 @@
       <c r="D41" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="E41" s="66"/>
+      <c r="E41" s="82"/>
       <c r="F41" s="3" t="s">
         <v>90</v>
       </c>
@@ -2507,7 +2516,7 @@
       <c r="D42" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E42" s="67"/>
+      <c r="E42" s="83"/>
       <c r="F42" s="3" t="s">
         <v>93</v>
       </c>
@@ -2522,26 +2531,26 @@
       <c r="K42" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="L42" s="100"/>
+      <c r="L42" s="64"/>
     </row>
     <row r="43" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D43" s="77" t="s">
+      <c r="D43" s="87" t="s">
         <v>95</v>
       </c>
-      <c r="E43" s="78"/>
-      <c r="F43" s="78"/>
-      <c r="G43" s="79"/>
+      <c r="E43" s="88"/>
+      <c r="F43" s="88"/>
+      <c r="G43" s="89"/>
       <c r="H43" s="22"/>
       <c r="I43" s="22"/>
       <c r="J43" s="22"/>
       <c r="K43" s="27"/>
-      <c r="L43" s="96"/>
+      <c r="L43" s="60"/>
     </row>
     <row r="44" spans="4:13" ht="30" x14ac:dyDescent="0.25">
       <c r="D44" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E44" s="65" t="s">
+      <c r="E44" s="81" t="s">
         <v>97</v>
       </c>
       <c r="F44" s="3" t="s">
@@ -2568,7 +2577,7 @@
       <c r="D45" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="E45" s="66"/>
+      <c r="E45" s="82"/>
       <c r="F45" s="3" t="s">
         <v>101</v>
       </c>
@@ -2595,24 +2604,24 @@
       <c r="D46" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="E46" s="67"/>
-      <c r="F46" s="88" t="s">
+      <c r="E46" s="83"/>
+      <c r="F46" s="52" t="s">
         <v>104</v>
       </c>
-      <c r="G46" s="89" t="s">
+      <c r="G46" s="53" t="s">
         <v>105</v>
       </c>
-      <c r="H46" s="92"/>
-      <c r="I46" s="103"/>
-      <c r="J46" s="92"/>
-      <c r="K46" s="104"/>
-      <c r="L46" s="97"/>
-    </row>
-    <row r="47" spans="4:13" s="109" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H46" s="56"/>
+      <c r="I46" s="65"/>
+      <c r="J46" s="56"/>
+      <c r="K46" s="66"/>
+      <c r="L46" s="61"/>
+    </row>
+    <row r="47" spans="4:13" s="71" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="D47" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="E47" s="62" t="s">
+      <c r="E47" s="90" t="s">
         <v>107</v>
       </c>
       <c r="F47" s="5" t="s">
@@ -2621,17 +2630,17 @@
       <c r="G47" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="H47" s="105" t="s">
+      <c r="H47" s="67" t="s">
         <v>210</v>
       </c>
-      <c r="I47" s="106">
+      <c r="I47" s="68">
         <v>42411</v>
       </c>
-      <c r="J47" s="105"/>
-      <c r="K47" s="107" t="s">
+      <c r="J47" s="67"/>
+      <c r="K47" s="69" t="s">
         <v>207</v>
       </c>
-      <c r="L47" s="108" t="s">
+      <c r="L47" s="70" t="s">
         <v>260</v>
       </c>
     </row>
@@ -2639,7 +2648,7 @@
       <c r="D48" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="E48" s="63"/>
+      <c r="E48" s="91"/>
       <c r="F48" s="5" t="s">
         <v>111</v>
       </c>
@@ -2656,7 +2665,7 @@
       <c r="K48" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="L48" s="98" t="s">
+      <c r="L48" s="62" t="s">
         <v>206</v>
       </c>
     </row>
@@ -2664,7 +2673,7 @@
       <c r="D49" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="E49" s="63"/>
+      <c r="E49" s="91"/>
       <c r="F49" s="3" t="s">
         <v>114</v>
       </c>
@@ -2683,7 +2692,7 @@
       <c r="K49" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="L49" s="98" t="s">
+      <c r="L49" s="62" t="s">
         <v>206</v>
       </c>
     </row>
@@ -2691,7 +2700,7 @@
       <c r="D50" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="E50" s="64"/>
+      <c r="E50" s="92"/>
       <c r="F50" s="3" t="s">
         <v>117</v>
       </c>
@@ -2710,7 +2719,7 @@
       <c r="K50" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="L50" s="98" t="s">
+      <c r="L50" s="62" t="s">
         <v>206</v>
       </c>
     </row>
@@ -2718,7 +2727,7 @@
       <c r="D51" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="E51" s="65" t="s">
+      <c r="E51" s="81" t="s">
         <v>120</v>
       </c>
       <c r="F51" s="7" t="s">
@@ -2735,13 +2744,13 @@
       <c r="K51" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="L51" s="100"/>
+      <c r="L51" s="64"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D52" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="E52" s="66"/>
+      <c r="E52" s="82"/>
       <c r="F52" s="3" t="s">
         <v>124</v>
       </c>
@@ -2756,13 +2765,13 @@
       <c r="K52" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="L52" s="100"/>
+      <c r="L52" s="64"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D53" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="E53" s="67"/>
+      <c r="E53" s="83"/>
       <c r="F53" s="3" t="s">
         <v>127</v>
       </c>
@@ -2777,30 +2786,30 @@
       <c r="K53" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="L53" s="100"/>
+      <c r="L53" s="64"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D54" s="77" t="s">
+      <c r="D54" s="87" t="s">
         <v>129</v>
       </c>
-      <c r="E54" s="78"/>
-      <c r="F54" s="78"/>
-      <c r="G54" s="79"/>
+      <c r="E54" s="88"/>
+      <c r="F54" s="88"/>
+      <c r="G54" s="89"/>
       <c r="H54" s="22"/>
       <c r="I54" s="22"/>
       <c r="J54" s="22"/>
       <c r="K54" s="12"/>
-      <c r="L54" s="96"/>
+      <c r="L54" s="60"/>
     </row>
     <row r="55" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="D55" s="4" t="s">
         <v>133</v>
       </c>
       <c r="E55" s="4"/>
-      <c r="F55" s="90" t="s">
+      <c r="F55" s="54" t="s">
         <v>131</v>
       </c>
-      <c r="G55" s="90" t="s">
+      <c r="G55" s="54" t="s">
         <v>132</v>
       </c>
       <c r="H55" s="26" t="s">
@@ -2815,7 +2824,7 @@
       <c r="K55" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="L55" s="99" t="s">
+      <c r="L55" s="63" t="s">
         <v>259</v>
       </c>
     </row>
@@ -2824,10 +2833,10 @@
         <v>137</v>
       </c>
       <c r="E56" s="4"/>
-      <c r="F56" s="91" t="s">
+      <c r="F56" s="55" t="s">
         <v>134</v>
       </c>
-      <c r="G56" s="90" t="s">
+      <c r="G56" s="54" t="s">
         <v>135</v>
       </c>
       <c r="H56" s="24" t="s">
@@ -2838,7 +2847,7 @@
       <c r="K56" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="L56" s="114"/>
+      <c r="L56" s="73"/>
     </row>
     <row r="57" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="D57" s="4" t="s">
@@ -2859,28 +2868,28 @@
       <c r="K57" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="L57" s="100" t="s">
+      <c r="L57" s="64" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D58" s="71" t="s">
+      <c r="D58" s="79" t="s">
         <v>136</v>
       </c>
-      <c r="E58" s="71"/>
-      <c r="F58" s="71"/>
-      <c r="G58" s="71"/>
+      <c r="E58" s="79"/>
+      <c r="F58" s="79"/>
+      <c r="G58" s="79"/>
       <c r="H58" s="22"/>
       <c r="I58" s="22"/>
       <c r="J58" s="22"/>
       <c r="K58" s="12"/>
-      <c r="L58" s="96"/>
+      <c r="L58" s="60"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D59" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="E59" s="68" t="s">
+      <c r="E59" s="96" t="s">
         <v>138</v>
       </c>
       <c r="F59" s="9" t="s">
@@ -2890,18 +2899,18 @@
       <c r="H59" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="I59" s="110"/>
-      <c r="J59" s="110"/>
+      <c r="I59" s="72"/>
+      <c r="J59" s="72"/>
       <c r="K59" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="L59" s="114"/>
+      <c r="L59" s="73"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D60" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="E60" s="69"/>
+      <c r="E60" s="97"/>
       <c r="F60" s="9" t="s">
         <v>141</v>
       </c>
@@ -2911,18 +2920,18 @@
       <c r="H60" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="I60" s="110"/>
-      <c r="J60" s="110"/>
+      <c r="I60" s="72"/>
+      <c r="J60" s="72"/>
       <c r="K60" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="L60" s="114"/>
+      <c r="L60" s="73"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D61" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="E61" s="69"/>
+      <c r="E61" s="97"/>
       <c r="F61" s="9" t="s">
         <v>144</v>
       </c>
@@ -2932,29 +2941,29 @@
       <c r="H61" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="I61" s="110"/>
-      <c r="J61" s="110"/>
+      <c r="I61" s="72"/>
+      <c r="J61" s="72"/>
       <c r="K61" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="L61" s="114"/>
+      <c r="L61" s="73"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D62" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="E62" s="69"/>
-      <c r="F62" s="88" t="s">
+      <c r="E62" s="97"/>
+      <c r="F62" s="52" t="s">
         <v>147</v>
       </c>
-      <c r="G62" s="88" t="s">
+      <c r="G62" s="52" t="s">
         <v>148</v>
       </c>
-      <c r="H62" s="92"/>
-      <c r="I62" s="92"/>
-      <c r="J62" s="92"/>
-      <c r="K62" s="93"/>
-      <c r="L62" s="97"/>
+      <c r="H62" s="56"/>
+      <c r="I62" s="56"/>
+      <c r="J62" s="56"/>
+      <c r="K62" s="57"/>
+      <c r="L62" s="61"/>
     </row>
     <row r="63" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
@@ -2963,7 +2972,7 @@
       <c r="D63" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="E63" s="69"/>
+      <c r="E63" s="97"/>
       <c r="F63" s="10" t="s">
         <v>150</v>
       </c>
@@ -2973,12 +2982,12 @@
       <c r="H63" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="I63" s="110"/>
-      <c r="J63" s="110"/>
+      <c r="I63" s="72"/>
+      <c r="J63" s="72"/>
       <c r="K63" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="L63" s="114"/>
+      <c r="L63" s="73"/>
     </row>
     <row r="64" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
@@ -2987,7 +2996,7 @@
       <c r="D64" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="E64" s="70"/>
+      <c r="E64" s="98"/>
       <c r="F64" s="10" t="s">
         <v>153</v>
       </c>
@@ -2997,12 +3006,12 @@
       <c r="H64" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="I64" s="110"/>
-      <c r="J64" s="110"/>
+      <c r="I64" s="72"/>
+      <c r="J64" s="72"/>
       <c r="K64" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="L64" s="114"/>
+      <c r="L64" s="73"/>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
@@ -3011,7 +3020,7 @@
       <c r="D65" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="E65" s="68" t="s">
+      <c r="E65" s="96" t="s">
         <v>156</v>
       </c>
       <c r="F65" s="9" t="s">
@@ -3040,7 +3049,7 @@
       <c r="D66" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="E66" s="69"/>
+      <c r="E66" s="97"/>
       <c r="F66" s="9" t="s">
         <v>160</v>
       </c>
@@ -3067,7 +3076,7 @@
       <c r="D67" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="E67" s="70"/>
+      <c r="E67" s="98"/>
       <c r="F67" s="10" t="s">
         <v>163</v>
       </c>
@@ -3086,13 +3095,13 @@
       <c r="K67" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="L67" s="114"/>
+      <c r="L67" s="73"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D68" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="E68" s="68" t="s">
+      <c r="E68" s="96" t="s">
         <v>166</v>
       </c>
       <c r="F68" s="9" t="s">
@@ -3113,13 +3122,13 @@
       <c r="K68" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="L68" s="98"/>
+      <c r="L68" s="62"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D69" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="E69" s="69"/>
+      <c r="E69" s="97"/>
       <c r="F69" s="9" t="s">
         <v>170</v>
       </c>
@@ -3138,13 +3147,13 @@
       <c r="K69" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="L69" s="98"/>
+      <c r="L69" s="62"/>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D70" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="E70" s="69"/>
+      <c r="E70" s="97"/>
       <c r="F70" s="9" t="s">
         <v>173</v>
       </c>
@@ -3159,34 +3168,34 @@
       <c r="K70" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="L70" s="98"/>
+      <c r="L70" s="62"/>
     </row>
     <row r="71" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D71" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="E71" s="69"/>
+      <c r="E71" s="97"/>
       <c r="F71" s="9" t="s">
         <v>213</v>
       </c>
       <c r="G71" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="H71" s="25" t="s">
-        <v>209</v>
-      </c>
-      <c r="I71" s="25"/>
-      <c r="J71" s="25"/>
-      <c r="K71" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="L71" s="98"/>
+      <c r="H71" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="I71" s="72"/>
+      <c r="J71" s="72"/>
+      <c r="K71" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="L71" s="62"/>
     </row>
     <row r="72" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D72" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="E72" s="70"/>
+      <c r="E72" s="98"/>
       <c r="F72" s="9" t="s">
         <v>211</v>
       </c>
@@ -3201,13 +3210,13 @@
       <c r="K72" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="L72" s="98"/>
+      <c r="L72" s="62"/>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D73" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="E73" s="68" t="s">
+      <c r="E73" s="96" t="s">
         <v>176</v>
       </c>
       <c r="F73" s="9" t="s">
@@ -3228,13 +3237,13 @@
       <c r="K73" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="L73" s="98"/>
+      <c r="L73" s="62"/>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D74" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="E74" s="69"/>
+      <c r="E74" s="97"/>
       <c r="F74" s="9" t="s">
         <v>180</v>
       </c>
@@ -3251,13 +3260,13 @@
       <c r="K74" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="L74" s="98"/>
+      <c r="L74" s="62"/>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D75" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="E75" s="70"/>
+      <c r="E75" s="98"/>
       <c r="F75" s="9" t="s">
         <v>183</v>
       </c>
@@ -3276,96 +3285,96 @@
       <c r="K75" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="L75" s="98"/>
+      <c r="L75" s="62"/>
     </row>
     <row r="76" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="D76" s="68" t="s">
+      <c r="D76" s="96" t="s">
         <v>217</v>
       </c>
-      <c r="E76" s="68" t="s">
+      <c r="E76" s="96" t="s">
         <v>186</v>
       </c>
-      <c r="F76" s="91" t="s">
+      <c r="F76" s="55" t="s">
         <v>187</v>
       </c>
-      <c r="G76" s="91" t="s">
+      <c r="G76" s="55" t="s">
         <v>188</v>
       </c>
-      <c r="H76" s="111" t="s">
+      <c r="H76" s="105" t="s">
         <v>210</v>
       </c>
-      <c r="I76" s="111"/>
-      <c r="J76" s="111"/>
-      <c r="K76" s="53" t="s">
+      <c r="I76" s="105"/>
+      <c r="J76" s="105"/>
+      <c r="K76" s="102" t="s">
         <v>208</v>
       </c>
-      <c r="L76" s="115"/>
+      <c r="L76" s="99"/>
     </row>
     <row r="77" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="D77" s="69"/>
-      <c r="E77" s="69"/>
-      <c r="F77" s="91" t="s">
+      <c r="D77" s="97"/>
+      <c r="E77" s="97"/>
+      <c r="F77" s="55" t="s">
         <v>189</v>
       </c>
-      <c r="G77" s="91" t="s">
+      <c r="G77" s="55" t="s">
         <v>190</v>
       </c>
-      <c r="H77" s="112"/>
-      <c r="I77" s="112"/>
-      <c r="J77" s="112"/>
-      <c r="K77" s="54"/>
-      <c r="L77" s="115"/>
+      <c r="H77" s="106"/>
+      <c r="I77" s="106"/>
+      <c r="J77" s="106"/>
+      <c r="K77" s="103"/>
+      <c r="L77" s="99"/>
     </row>
     <row r="78" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="D78" s="69"/>
-      <c r="E78" s="69"/>
-      <c r="F78" s="91" t="s">
+      <c r="D78" s="97"/>
+      <c r="E78" s="97"/>
+      <c r="F78" s="55" t="s">
         <v>191</v>
       </c>
-      <c r="G78" s="91" t="s">
+      <c r="G78" s="55" t="s">
         <v>192</v>
       </c>
-      <c r="H78" s="112"/>
-      <c r="I78" s="112"/>
-      <c r="J78" s="112"/>
-      <c r="K78" s="54"/>
-      <c r="L78" s="115"/>
+      <c r="H78" s="106"/>
+      <c r="I78" s="106"/>
+      <c r="J78" s="106"/>
+      <c r="K78" s="103"/>
+      <c r="L78" s="99"/>
     </row>
     <row r="79" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="D79" s="69"/>
-      <c r="E79" s="69"/>
-      <c r="F79" s="91" t="s">
+      <c r="D79" s="97"/>
+      <c r="E79" s="97"/>
+      <c r="F79" s="55" t="s">
         <v>193</v>
       </c>
-      <c r="G79" s="91" t="s">
+      <c r="G79" s="55" t="s">
         <v>194</v>
       </c>
-      <c r="H79" s="112"/>
-      <c r="I79" s="112"/>
-      <c r="J79" s="112"/>
-      <c r="K79" s="54"/>
-      <c r="L79" s="115"/>
+      <c r="H79" s="106"/>
+      <c r="I79" s="106"/>
+      <c r="J79" s="106"/>
+      <c r="K79" s="103"/>
+      <c r="L79" s="99"/>
     </row>
     <row r="80" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="D80" s="70"/>
-      <c r="E80" s="70"/>
-      <c r="F80" s="91" t="s">
+      <c r="D80" s="98"/>
+      <c r="E80" s="98"/>
+      <c r="F80" s="55" t="s">
         <v>195</v>
       </c>
-      <c r="G80" s="90" t="s">
+      <c r="G80" s="54" t="s">
         <v>196</v>
       </c>
-      <c r="H80" s="113"/>
-      <c r="I80" s="113"/>
-      <c r="J80" s="113"/>
-      <c r="K80" s="55"/>
-      <c r="L80" s="115"/>
+      <c r="H80" s="107"/>
+      <c r="I80" s="107"/>
+      <c r="J80" s="107"/>
+      <c r="K80" s="104"/>
+      <c r="L80" s="99"/>
     </row>
     <row r="81" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D81" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="E81" s="72" t="s">
+      <c r="E81" s="78" t="s">
         <v>251</v>
       </c>
       <c r="F81" s="10" t="s">
@@ -3384,13 +3393,13 @@
       <c r="K81" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="L81" s="98"/>
+      <c r="L81" s="62"/>
     </row>
     <row r="82" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D82" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="E82" s="72"/>
+      <c r="E82" s="78"/>
       <c r="F82" s="10" t="s">
         <v>255</v>
       </c>
@@ -3407,11 +3416,30 @@
       <c r="K82" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="L82" s="98"/>
+      <c r="L82" s="62"/>
     </row>
   </sheetData>
   <autoFilter ref="H10:H82"/>
   <mergeCells count="35">
+    <mergeCell ref="L76:L80"/>
+    <mergeCell ref="L23:L24"/>
+    <mergeCell ref="K76:K80"/>
+    <mergeCell ref="H76:H80"/>
+    <mergeCell ref="I76:I80"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="K23:K24"/>
+    <mergeCell ref="J76:J80"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="E47:E50"/>
+    <mergeCell ref="E44:E46"/>
+    <mergeCell ref="E51:E53"/>
+    <mergeCell ref="E73:E75"/>
+    <mergeCell ref="E76:E80"/>
+    <mergeCell ref="D58:G58"/>
+    <mergeCell ref="E59:E64"/>
+    <mergeCell ref="D76:D80"/>
+    <mergeCell ref="E68:E72"/>
+    <mergeCell ref="E65:E67"/>
     <mergeCell ref="E81:E82"/>
     <mergeCell ref="D11:G11"/>
     <mergeCell ref="D12:G12"/>
@@ -3428,25 +3456,6 @@
     <mergeCell ref="E28:E31"/>
     <mergeCell ref="E37:E39"/>
     <mergeCell ref="E40:E42"/>
-    <mergeCell ref="E47:E50"/>
-    <mergeCell ref="E44:E46"/>
-    <mergeCell ref="E51:E53"/>
-    <mergeCell ref="E73:E75"/>
-    <mergeCell ref="E76:E80"/>
-    <mergeCell ref="D58:G58"/>
-    <mergeCell ref="E59:E64"/>
-    <mergeCell ref="D76:D80"/>
-    <mergeCell ref="E68:E72"/>
-    <mergeCell ref="E65:E67"/>
-    <mergeCell ref="K76:K80"/>
-    <mergeCell ref="H76:H80"/>
-    <mergeCell ref="I76:I80"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="K23:K24"/>
-    <mergeCell ref="J76:J80"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="L76:L80"/>
-    <mergeCell ref="L23:L24"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:I5">
     <cfRule type="colorScale" priority="1">
@@ -3467,7 +3476,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H81:H82 H56:H57 H59:H76">
       <formula1>$A$63:$A$65</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L65:L66 H3:H5 K13:K23 K81:K82 L48:L50 K25:K76 L40:L41 L44:L45">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L65:L66 H3:H5 K13:K23 K81:K82 L48:L50 L44:L45 L40:L41 K25:K76">
       <formula1>$B$18:$B$20</formula1>
     </dataValidation>
   </dataValidations>
@@ -3516,16 +3525,16 @@
       <c r="I4" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="K4" s="52" t="s">
+      <c r="K4" s="119" t="s">
         <v>215</v>
       </c>
-      <c r="L4" s="52"/>
+      <c r="L4" s="119"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="D5" s="68" t="s">
+      <c r="D5" s="96" t="s">
         <v>231</v>
       </c>
       <c r="E5" s="9" t="s">
@@ -3555,7 +3564,7 @@
       <c r="B6" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="D6" s="69"/>
+      <c r="D6" s="97"/>
       <c r="E6" s="9" t="s">
         <v>233</v>
       </c>
@@ -3579,7 +3588,7 @@
       <c r="B7" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="D7" s="83" t="s">
+      <c r="D7" s="114" t="s">
         <v>222</v>
       </c>
       <c r="E7" s="33" t="s">
@@ -3605,7 +3614,7 @@
       <c r="B8" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="D8" s="84"/>
+      <c r="D8" s="115"/>
       <c r="E8" s="33" t="s">
         <v>225</v>
       </c>
@@ -3621,7 +3630,7 @@
       <c r="L8" s="39"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D9" s="85"/>
+      <c r="D9" s="116"/>
       <c r="E9" s="33" t="s">
         <v>226</v>
       </c>
@@ -3637,7 +3646,7 @@
       <c r="L9" s="39"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D10" s="86" t="s">
+      <c r="D10" s="117" t="s">
         <v>227</v>
       </c>
       <c r="E10" s="34" t="s">
@@ -3658,7 +3667,7 @@
       <c r="B11" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="D11" s="87"/>
+      <c r="D11" s="118"/>
       <c r="E11" s="34" t="s">
         <v>234</v>
       </c>
@@ -3775,10 +3784,10 @@
       <c r="H4" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="J4" s="52" t="s">
+      <c r="J4" s="119" t="s">
         <v>215</v>
       </c>
-      <c r="K4" s="52"/>
+      <c r="K4" s="119"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">

</xml_diff>